<commit_message>
Added Condition and Device
</commit_message>
<xml_diff>
--- a/maps/xtehr2zibs/Device.xlsx
+++ b/maps/xtehr2zibs/Device.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\mgraauw\eu-nl-compared\maps\xtehr2zibs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B92A2F7-8C45-45EB-8A6E-0DCBE6849E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564C2153-AFED-4571-8358-78BE00968E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12585" yWindow="-21600" windowWidth="17415" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-12585" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,161 +20,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="65">
-  <si>
-    <t>short</t>
-  </si>
-  <si>
-    <t>definition</t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>card.</t>
-  </si>
-  <si>
-    <t>binding</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>EHDSDevice</t>
   </si>
   <si>
-    <t>Device model</t>
-  </si>
-  <si>
-    <t>C.12 - EHDS refined base model for Device information</t>
-  </si>
-  <si>
-    <t>0..*</t>
-  </si>
-  <si>
     <t>EHDSDevice.identifier</t>
   </si>
   <si>
-    <t>C.12.1 - Identifier</t>
-  </si>
-  <si>
-    <t>An identifier of the device which is unique within in a defined scope. Multiple identifiers can be used.</t>
-  </si>
-  <si>
-    <t>Identifier</t>
-  </si>
-  <si>
-    <t>1..*</t>
-  </si>
-  <si>
     <t>EHDSDevice.manufacturer</t>
   </si>
   <si>
-    <t>C.12.2 - Manufacturer</t>
-  </si>
-  <si>
-    <t>Name of device manufacturer</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>0..1</t>
-  </si>
-  <si>
     <t>EHDSDevice.manufactureDate</t>
   </si>
   <si>
-    <t>C.12.3 - Manufacture date</t>
-  </si>
-  <si>
-    <t>The date and time when the device was manufactured</t>
-  </si>
-  <si>
-    <t>dateTime</t>
-  </si>
-  <si>
     <t>EHDSDevice.expiryDate</t>
   </si>
   <si>
-    <t>C.12.4 - Expiry date</t>
-  </si>
-  <si>
-    <t>The date and time beyond which this device is no longer valid or should not be used (if applicable).</t>
-  </si>
-  <si>
     <t>EHDSDevice.lotNumber</t>
   </si>
   <si>
-    <t>C.12.5 - Lot number</t>
-  </si>
-  <si>
-    <t>Lot number of manufacture</t>
-  </si>
-  <si>
     <t>EHDSDevice.serialNumber</t>
   </si>
   <si>
-    <t>C.12.6 - Serial number</t>
-  </si>
-  <si>
-    <t>Serial number assigned by the manufacturer</t>
-  </si>
-  <si>
     <t>EHDSDevice.name</t>
   </si>
   <si>
-    <t>C.12.7 - Name</t>
-  </si>
-  <si>
-    <t>The name and name type of the device as known to the manufacturer and/or patient</t>
-  </si>
-  <si>
     <t>EHDSDevice.modelNumber</t>
   </si>
   <si>
-    <t>C.12.8 - Model number</t>
-  </si>
-  <si>
-    <t>The manufacturer's model number for the device</t>
-  </si>
-  <si>
     <t>EHDSDevice.version</t>
   </si>
   <si>
-    <t>C.12.9 - Version</t>
-  </si>
-  <si>
-    <t>The actual design of the device or software version running on the device</t>
-  </si>
-  <si>
     <t>EHDSDevice.type</t>
   </si>
   <si>
-    <t>C.12.10 - Type</t>
-  </si>
-  <si>
-    <t>Device type</t>
-  </si>
-  <si>
-    <t>CodeableConcept</t>
-  </si>
-  <si>
-    <t>{'strength': 'preferred', 'description': 'SNOMED CT, EMDN'}</t>
-  </si>
-  <si>
     <t>EHDSDevice.note</t>
   </si>
   <si>
-    <t>C.12.11 - Note</t>
-  </si>
-  <si>
-    <t>Device notes and comments</t>
-  </si>
-  <si>
-    <t>Narrative</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
     <t>MedicalDevice</t>
   </si>
   <si>
@@ -187,18 +70,6 @@
     <t>MedicalDevice.Product.ProductType</t>
   </si>
   <si>
-    <t>MedicalDevice.AnatomicalLocation.ProductType</t>
-  </si>
-  <si>
-    <t>MedicalDevice.StartDate.ProductType</t>
-  </si>
-  <si>
-    <t>MedicalDevice.EindDatum.ProductType</t>
-  </si>
-  <si>
-    <t>MedicalDevice.Comment.ProductType</t>
-  </si>
-  <si>
     <t>xtehr</t>
   </si>
   <si>
@@ -215,6 +86,18 @@
   </si>
   <si>
     <t>MedicalDevice.HealthProfessional</t>
+  </si>
+  <si>
+    <t>MedicalDevice.EindDatum</t>
+  </si>
+  <si>
+    <t>MedicalDevice.AnatomicalLocation</t>
+  </si>
+  <si>
+    <t>MedicalDevice.Comment</t>
+  </si>
+  <si>
+    <t>MedicalDevice.StartDate</t>
   </si>
 </sst>
 </file>
@@ -577,308 +460,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.42578125" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" customWidth="1"/>
-    <col min="5" max="5" width="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>